<commit_message>
Alteradas especificações de Use Case
</commit_message>
<xml_diff>
--- a/Fase2/UML/Especificação de Use Cases/Adicionar Pintor.xlsx
+++ b/Fase2/UML/Especificação de Use Cases/Adicionar Pintor.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaop\Google Drive\Universidade\3º + 2º Ano_\2º Semestre\LI4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaop\OneDrive\Documents\GitHub\li4-17-18\Fase2\UML\Especificação de Use Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E97594-6211-4AD6-9E16-BAFBB5778265}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C92E58E9-BCC4-444F-8938-87E9880A8FCC}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795" xr2:uid="{B5A471B3-53AC-4CFD-8B13-ED91E0AC6FA3}"/>
   </bookViews>
@@ -130,11 +130,11 @@
     <t xml:space="preserve">Adiciona Pintor a Lista de Pintores  </t>
   </si>
   <si>
+    <t>Indica que o pintor já existe no sistema</t>
+  </si>
+  <si>
     <t>Excepção 1               (passo 2)
-[Pintor já existe no sistema]</t>
-  </si>
-  <si>
-    <t>Indica que o pintor já existe no sistema</t>
+[Pintor Existente]</t>
   </si>
 </sst>
 </file>
@@ -526,7 +526,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -682,14 +682,14 @@
     </row>
     <row r="16" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Acrescentado especificações atribuídas ao Cesário e ao Tiago
</commit_message>
<xml_diff>
--- a/Fase2/UML/Especificação de Use Cases/Adicionar Pintor.xlsx
+++ b/Fase2/UML/Especificação de Use Cases/Adicionar Pintor.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaop\OneDrive\Documents\GitHub\li4-17-18\Fase2\UML\Especificação de Use Cases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaop\Google Drive\Universidade\3º + 2º Ano_\2º Semestre\LI4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C92E58E9-BCC4-444F-8938-87E9880A8FCC}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E97594-6211-4AD6-9E16-BAFBB5778265}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795" xr2:uid="{B5A471B3-53AC-4CFD-8B13-ED91E0AC6FA3}"/>
   </bookViews>
@@ -130,11 +130,11 @@
     <t xml:space="preserve">Adiciona Pintor a Lista de Pintores  </t>
   </si>
   <si>
+    <t>Excepção 1               (passo 2)
+[Pintor já existe no sistema]</t>
+  </si>
+  <si>
     <t>Indica que o pintor já existe no sistema</t>
-  </si>
-  <si>
-    <t>Excepção 1               (passo 2)
-[Pintor Existente]</t>
   </si>
 </sst>
 </file>
@@ -526,7 +526,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -682,14 +682,14 @@
     </row>
     <row r="16" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Alterado Diagrama de Sequência Adicionar Pintor
</commit_message>
<xml_diff>
--- a/Fase2/UML/Especificação de Use Cases/Adicionar Pintor.xlsx
+++ b/Fase2/UML/Especificação de Use Cases/Adicionar Pintor.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaop\Google Drive\Universidade\3º + 2º Ano_\2º Semestre\LI4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaop\Google Drive\Universidade\3º + 2º Ano_\2º Semestre\LI4\Especificação de Use Cases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E97594-6211-4AD6-9E16-BAFBB5778265}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F8E546-9293-46F6-8A12-68C3D6A08724}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795" xr2:uid="{B5A471B3-53AC-4CFD-8B13-ED91E0AC6FA3}"/>
   </bookViews>
@@ -124,9 +124,6 @@
     <t>Incrementa número de Pintores</t>
   </si>
   <si>
-    <t>Devolve Dados de autenticação do Pintor</t>
-  </si>
-  <si>
     <t xml:space="preserve">Adiciona Pintor a Lista de Pintores  </t>
   </si>
   <si>
@@ -135,6 +132,9 @@
   </si>
   <si>
     <t>Indica que o pintor já existe no sistema</t>
+  </si>
+  <si>
+    <t>Devolve dados de autenticação do pintor</t>
   </si>
 </sst>
 </file>
@@ -526,7 +526,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,7 +667,7 @@
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -682,14 +682,14 @@
     </row>
     <row r="16" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Relatorio com parte da Nadine, analise de requisitos e modelo concetual da BD acabados
</commit_message>
<xml_diff>
--- a/Fase2/UML/Especificação de Use Cases/Adicionar Pintor.xlsx
+++ b/Fase2/UML/Especificação de Use Cases/Adicionar Pintor.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaop\Google Drive\Universidade\3º + 2º Ano_\2º Semestre\LI4\Especificação de Use Cases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaop\Google Drive\Universidade\3º + 2º Ano_\2º Semestre\LI4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54F8E546-9293-46F6-8A12-68C3D6A08724}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E97594-6211-4AD6-9E16-BAFBB5778265}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795" xr2:uid="{B5A471B3-53AC-4CFD-8B13-ED91E0AC6FA3}"/>
   </bookViews>
@@ -124,6 +124,9 @@
     <t>Incrementa número de Pintores</t>
   </si>
   <si>
+    <t>Devolve Dados de autenticação do Pintor</t>
+  </si>
+  <si>
     <t xml:space="preserve">Adiciona Pintor a Lista de Pintores  </t>
   </si>
   <si>
@@ -132,9 +135,6 @@
   </si>
   <si>
     <t>Indica que o pintor já existe no sistema</t>
-  </si>
-  <si>
-    <t>Devolve dados de autenticação do pintor</t>
   </si>
 </sst>
 </file>
@@ -526,7 +526,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -667,7 +667,7 @@
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -682,14 +682,14 @@
     </row>
     <row r="16" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>